<commit_message>
feat: added option to see overflow answer options
</commit_message>
<xml_diff>
--- a/data/stimuli_en/multipleye_stimuli_experiment_en.xlsx
+++ b/data/stimuli_en/multipleye_stimuli_experiment_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_308f\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_en/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{2094D4B0-1619-4621-807D-BE7CF5FE5B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF98D675-3E15-4C8C-9606-80B88EBCBFF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BBA8C3-76F1-A14A-A7CA-AE8500130342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="15480" windowHeight="11640" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="PopSci_MultiplEYE_EN_example_st" sheetId="2" r:id="rId1"/>
@@ -616,7 +616,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -686,7 +686,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1000,26 +1000,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9016B68B-E770-4A04-A8EB-C009482E3DEC}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="81.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="81.28515625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="81.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="73.28515625" style="1" customWidth="1"/>
-    <col min="12" max="16" width="81.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="26" width="81.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.33203125" style="1" customWidth="1"/>
+    <col min="9" max="10" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="73.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16" width="81.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="26" width="81.1640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1100,7 @@
       </c>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="91.5">
+    <row r="2" spans="1:27" ht="80" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="122.25" customHeight="1">
+    <row r="3" spans="1:27" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="121.5">
+    <row r="4" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="106.5">
+    <row r="5" spans="1:27" ht="96" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="152.25">
+    <row r="6" spans="1:27" ht="144" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="106.5">
+    <row r="7" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="121.5">
+    <row r="8" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="137.25">
+    <row r="9" spans="1:27" ht="128" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" ht="106.5">
+    <row r="10" spans="1:27" ht="96" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1433,7 +1433,7 @@
       </c>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="137.25">
+    <row r="11" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="AA11" s="3"/>
     </row>
-    <row r="12" spans="1:27" ht="91.5">
+    <row r="12" spans="1:27" ht="80" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="121.5">
+    <row r="13" spans="1:27" ht="96" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="137.25">
+    <row r="14" spans="1:27" ht="128" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1664,60 +1664,60 @@
       </c>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I16" s="5"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="18" spans="5:19">
+    <row r="18" spans="5:19" x14ac:dyDescent="0.2">
       <c r="N18" s="2"/>
       <c r="S18" s="2"/>
     </row>
-    <row r="20" spans="5:19">
+    <row r="20" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F20" s="2"/>
       <c r="N20" s="2"/>
       <c r="S20" s="2"/>
     </row>
-    <row r="21" spans="5:19">
+    <row r="21" spans="5:19" x14ac:dyDescent="0.2">
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="5:19">
+    <row r="22" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F22" s="2"/>
       <c r="I22" s="2"/>
       <c r="N22" s="2"/>
       <c r="S22" s="2"/>
     </row>
-    <row r="23" spans="5:19">
+    <row r="23" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="5:19">
+    <row r="24" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F24" s="2"/>
       <c r="I24" s="2"/>
       <c r="N24" s="2"/>
       <c r="S24" s="2"/>
     </row>
-    <row r="25" spans="5:19">
+    <row r="25" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="5:19">
+    <row r="26" spans="5:19" x14ac:dyDescent="0.2">
       <c r="F26" s="2"/>
       <c r="I26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="5:19">
+    <row r="27" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:19">
+    <row r="28" spans="5:19" x14ac:dyDescent="0.2">
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="5:19">
+    <row r="29" spans="5:19" x14ac:dyDescent="0.2">
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="5:19">
+    <row r="30" spans="5:19" x14ac:dyDescent="0.2">
       <c r="I30" s="2"/>
     </row>
   </sheetData>
@@ -1736,5 +1736,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>